<commit_message>
ultimos diccionarios pero hace falta revisar todos
</commit_message>
<xml_diff>
--- a/04_Entregable 2/previo/resumen_bdd_2025-03-25_AG.xlsx
+++ b/04_Entregable 2/previo/resumen_bdd_2025-03-25_AG.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angleito\Documents\Consultorías\wcs\04_Entregable 2\previo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MAG\personal\consultorías\wcs\04_Entregable 2\previo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -273,7 +273,7 @@
     <t>Como hoja 2 de 06 pero sin celdas combinadas</t>
   </si>
   <si>
-    <t>Como hoja 1 de 06 pero sin celdas combinadas</t>
+    <t>Tiene cuatro hojas, BD_2022 tiene la información de BD_OR_2022 y más registros, las hojas TD_2022 y Hoja 1 son tablas dinámicas y gráficos, se realiza unicamente el diccionario de BD_2022</t>
   </si>
 </sst>
 </file>
@@ -651,7 +651,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +894,7 @@
       <c r="F9" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="H9" t="s">
@@ -946,7 +946,7 @@
       <c r="F11" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="H11" t="s">

</xml_diff>